<commit_message>
Cleaned up code a bit
I cleaned up some of AHP and ELECTRE to make it easier to read and less lines.
</commit_message>
<xml_diff>
--- a/dmsan/results/RESULTS_AHP_ELECTRE.xlsx
+++ b/dmsan/results/RESULTS_AHP_ELECTRE.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="38">
   <si>
     <t>T1</t>
   </si>
@@ -113,9 +113,6 @@
   </si>
   <si>
     <t>S12</t>
-  </si>
-  <si>
-    <t>sum</t>
   </si>
   <si>
     <t>D12</t>
@@ -1208,13 +1205,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="B1" s="1">
         <v>0</v>
       </c>
@@ -1224,11 +1221,8 @@
       <c r="D1" s="1">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>32</v>
-      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1241,11 +1235,8 @@
       <c r="D2">
         <v>3.348484488655513</v>
       </c>
-      <c r="E2">
-        <v>5.59515409507091</v>
-      </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1258,11 +1249,8 @@
       <c r="D3">
         <v>3.449599991972164</v>
       </c>
-      <c r="E3">
-        <v>8.033254160183025</v>
-      </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1274,9 +1262,6 @@
       </c>
       <c r="D4">
         <v>0</v>
-      </c>
-      <c r="E4">
-        <v>5.917516680809346</v>
       </c>
     </row>
   </sheetData>
@@ -1392,7 +1377,7 @@
     </row>
     <row r="2" spans="1:33">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1493,7 +1478,7 @@
     </row>
     <row r="3" spans="1:33">
       <c r="A3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3">
         <v>0.004223085072947563</v>
@@ -1594,7 +1579,7 @@
     </row>
     <row r="4" spans="1:33">
       <c r="A4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1695,7 +1680,7 @@
     </row>
     <row r="5" spans="1:33">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5">
         <v>0.004223085072947563</v>
@@ -1796,7 +1781,7 @@
     </row>
     <row r="6" spans="1:33">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6">
         <v>0.004223085072947563</v>
@@ -1897,7 +1882,7 @@
     </row>
     <row r="7" spans="1:33">
       <c r="A7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7">
         <v>0.004223085072947563</v>

</xml_diff>